<commit_message>
CAN2-31 tx priority reqs generated ready for review cr1
</commit_message>
<xml_diff>
--- a/CAN_Controller_Requirements_ColinFritz.xlsx
+++ b/CAN_Controller_Requirements_ColinFritz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfritz/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15822F53-FA43-2C47-8FAC-850953F90D7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF883F0-C86D-DD43-8651-A3ACCC645E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="460" windowWidth="32980" windowHeight="18680" activeTab="1" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
+    <workbookView xWindow="6320" yWindow="460" windowWidth="32980" windowHeight="18680" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tx_Priority_Logic" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Function</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>The module shall transmit or discard messages in the order they are received via i_rx_message[127:0]</t>
+  </si>
+  <si>
+    <t>TxPL_PRIORITY_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall implement full and empty flags for indicating the occupancy of the internal register.  </t>
   </si>
 </sst>
 </file>
@@ -392,16 +398,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -429,6 +432,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5DD9F9-33F5-AB4F-8754-0782077CDA3E}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,7 +771,7 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -775,10 +782,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -789,8 +796,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -801,8 +808,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -811,18 +818,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -833,8 +840,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -843,18 +850,18 @@
       </c>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="8" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="7" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:4" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -864,26 +871,43 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+    <row r="10" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="17"/>
     </row>
     <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="17"/>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="17"/>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -894,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055E712C-2DEB-9048-A84E-E3F1D6680CEE}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -908,24 +932,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -936,8 +960,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -948,8 +972,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -960,8 +984,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2" t="s">
         <v>36</v>
       </c>
@@ -970,8 +994,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>37</v>
       </c>
@@ -980,8 +1004,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
         <v>38</v>
       </c>
@@ -990,8 +1014,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="2" t="s">
         <v>39</v>
       </c>
@@ -1000,18 +1024,18 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1022,8 +1046,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="2" t="s">
         <v>50</v>
       </c>
@@ -1032,8 +1056,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1042,8 +1066,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="2" t="s">
         <v>52</v>
       </c>
@@ -1052,8 +1076,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="2" t="s">
         <v>53</v>
       </c>
@@ -1062,18 +1086,18 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1084,8 +1108,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2" t="s">
         <v>60</v>
       </c>
@@ -1094,19 +1118,19 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="8" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="8" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="5" t="s">

</xml_diff>

<commit_message>
CAN2-27 CAN2-30  acceptance filter and TX priority logic reg rev1
</commit_message>
<xml_diff>
--- a/CAN_Controller_Requirements_ColinFritz.xlsx
+++ b/CAN_Controller_Requirements_ColinFritz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfritz/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF883F0-C86D-DD43-8651-A3ACCC645E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7A7CB6-20CC-704F-88C7-076468AC293F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="460" windowWidth="32980" windowHeight="18680" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="32620" windowHeight="18680" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tx_Priority_Logic" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="143">
   <si>
     <t>Function</t>
   </si>
@@ -123,27 +123,9 @@
     <t>ACCEPT_INIT_01</t>
   </si>
   <si>
-    <t>If i_reset is high the module shall set o_rx_w_en low, o_acfbsy low, and o_rx_fifo_w_data[127:0]</t>
-  </si>
-  <si>
     <t xml:space="preserve">REC </t>
   </si>
   <si>
-    <t xml:space="preserve">If i_uaf1 is high the module shall mask the i_rx_message[31:0] with the contents of afmr1 and store the result separately in internal register1 for filtering by ID.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">If i_uaf2 is high the module shall mask the i_rx_message[31:0] with the contents of afmr2 and store the result separately in internal register2 for filtering by ID.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">If i_uaf3 is high the module shall mask the i_rx_message[31:0] with the contents of afmr3 and store the result separately in internal register3 for filtering by ID.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">If i_uaf4 is high the module shall mask the i_rx_message[31:0] with the contents of afmr4 and store the result separately in internal register4 for filtering by ID.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall mask i_rx_message[31:0] with the corresponding bits of i_afmr1,2,3,4[31:0];  afmr1,2,3,4[0] masks i_rx_message[0] and so on.  </t>
-  </si>
-  <si>
     <t>ACCEPT_MASKMSG_02</t>
   </si>
   <si>
@@ -162,6 +144,15 @@
     <t>ACCEPT_MASKID_06</t>
   </si>
   <si>
+    <t>ACCEPT_MASKID_07</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKID_08</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKID_09</t>
+  </si>
+  <si>
     <t>MASKMSG</t>
   </si>
   <si>
@@ -174,13 +165,16 @@
     <t>If i_uaf2 is high The module shall mask i_afir2[31:0] with the contents of afmr2 and store the result in internal register6</t>
   </si>
   <si>
+    <t>ACCEPT_MASKID_10</t>
+  </si>
+  <si>
     <t>If i_uaf3 is high The module shall mask i_afir3[31:0] with the contents of afmr3 and store the result in internal register7</t>
   </si>
   <si>
     <t>If i_uaf4 is high The module shall mask i_afir4[31:0] with the contents of afmr3 and store the result in internal register8</t>
   </si>
   <si>
-    <t xml:space="preserve">The module shall mask i_afir1,2,3,4[31:0] with the corresponding bits of i_afmr1,2,3,4[31:0];  afmr1,2,3,4[0] masks i_afir1,2,3,4[0] and so on.  </t>
+    <t>ACCEPT_MASKID_11</t>
   </si>
   <si>
     <t>ACCEPT_MASKID_01</t>
@@ -201,15 +195,6 @@
     <t>ACCEPT_MASKMSG_01</t>
   </si>
   <si>
-    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKID_01-05 within 20 i_sys_clk cycles starting with the rising edge of i_sys_clk recognizing i_uaf1,2,3,or 4 as high.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKMSG_01-05 within 20 i_can_clk cycles starting with the rising edge of i_can_clk recognizing i_uaf1,2,3,or 4 as high.  </t>
-  </si>
-  <si>
-    <t>if i_can_ready is high the module shall accept i_rx_message[127:0] on the next rising edge of i_can_clk and mask the contents according to ACCEPT_MASKMSG_01-05 before storing the result(s) in internal register(s) for filtering by ID</t>
-  </si>
-  <si>
     <t>ACCEPT_TRANSMIT_01</t>
   </si>
   <si>
@@ -225,22 +210,259 @@
     <t xml:space="preserve">If i_rx_full is high the module shall not pulse o_rx_w_en </t>
   </si>
   <si>
-    <t>If i_rx_full is low the module shall transmit messages via a one clock cycle pulse of o_rx_w_en.  (low high low pulse)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If i_uaf1,2,3, or 4 is high then the module shall set o_acfbsy high, otherwise if all i_uaf1,2,3 and 4 are low o_acfbsy shall be set low.  </t>
-  </si>
-  <si>
     <t>ACCEPT_TRANSMIT_04</t>
   </si>
   <si>
-    <t>The module shall transmit or discard messages in the order they are received via i_rx_message[127:0]</t>
-  </si>
-  <si>
     <t>TxPL_PRIORITY_02</t>
   </si>
   <si>
     <t xml:space="preserve">The module shall implement full and empty flags for indicating the occupancy of the internal register.  </t>
+  </si>
+  <si>
+    <t>ACCEPT_INIT_02</t>
+  </si>
+  <si>
+    <t>ACCEPT_INIT_03</t>
+  </si>
+  <si>
+    <t>If i_reset is high the module shall set o_rx_w_en low</t>
+  </si>
+  <si>
+    <t>If i_reset is high the module shall set o_acfbsy low</t>
+  </si>
+  <si>
+    <t>If i_reset is high the module shall set o_rx_fifo_w_data[127:0]</t>
+  </si>
+  <si>
+    <t>If i_rx_full is low the module shall transmit messages via a one clock cycle pulse of o_rx_w_en</t>
+  </si>
+  <si>
+    <t>The module shall mask i_afir4[31:0] with the corresponding bits of i_afmr4[31:0];  afmr4[0] masks i_afir4[0] and so on in ACCEPT_MASKID_04</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKMSG_07</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKMSG_08</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKMSG_09</t>
+  </si>
+  <si>
+    <t>The module shall mask i_afir1[31:0] with the corresponding bits of i_afmr1[31:0];  afmr1[0] masks i_afir1[0] and so on in ACCEPT_MASKID_01</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKID_12</t>
+  </si>
+  <si>
+    <t>The module shall mask i_afir3[31:0] with the corresponding bits of i_afmr3[31:0];  afmr3[0] masks i_afir3[0] and so on in ACCEPT_MASKID_03</t>
+  </si>
+  <si>
+    <t>The module shall mask i_afir2[31:0] with the corresponding bits of i_afmr2[31:0];  afmr2[0] masks i_afir2[0] and so on in ACCEPT_MASKID_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKID_01 -08 within 20 i_sys_clk cycles starting with the rising edge of i_sys_clk recognizing i_uaf1 as high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKID_01-08 within 20 i_sys_clk cycles starting with the rising edge of i_sys_clk recognizing i_uaf2 as high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKID_01-08 within 20 i_sys_clk cycles starting with the rising edge of i_sys_clk recognizing i_uaf3 as high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKID_01-08 within 20 i_sys_clk cycles starting with the rising edge of i_sys_clk recognizing i_uaf4 as high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If i_uaf1 is high the module shall mask the i_rx_message[127:96] with the contents of afmr1 and store the result separately in internal register1 for filtering by ID.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If i_uaf2 is high the module shall mask the i_rx_message[127:96] with the contents of afmr2 and store the result separately in internal register2 for filtering by ID.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If i_uaf3 is high the module shall mask the i_rx_message[127:96] with the contents of afmr3 and store the result separately in internal register3 for filtering by ID.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If i_uaf4 is high the module shall mask the i_rx_message[127:96] with the contents of afmr4 and store the result separately in internal register4 for filtering by ID.  </t>
+  </si>
+  <si>
+    <t>The module shall mask i_rx_message[127:96] with the corresponding bits of i_afmr1[31:0];  afmr1[0] masks i_rx_message[96] and so on in ACCEPT_MASKMSG_01</t>
+  </si>
+  <si>
+    <t>The module shall mask i_rx_message[127:96] with the corresponding bits of i_afmr2[31:0];  afmr2[0] masks i_rx_message[96] and so on in ACCEPT_MASKMSG_02</t>
+  </si>
+  <si>
+    <t>The module shall mask i_rx_message[127:96] with the corresponding bits of i_afmr3[31:0];  afmr3[0] masks i_rx_message[96] and so on in ACCEPT_MASKMSG_03</t>
+  </si>
+  <si>
+    <t>The module shall mask i_rx_message[127:96] with the corresponding bits of i_afmr4[31:0];  afmr4[0] masks i_rx_message[96] and so on in ACCEPT_MASKMSG_04</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKMSG_10</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKMSG_11</t>
+  </si>
+  <si>
+    <t>ACCEPT_MASKMSG_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKMSG_01 and  ACCEPT_MASKMSG_05 within 20 i_can_clk cycles starting with the rising edge of i_can_clk recognizing i_uaf1 as high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKMSG_02 and  ACCEPT_MASKMSG_06 within 20 i_can_clk cycles starting with the rising edge of i_can_clk recognizing i_uaf2 as high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKMSG_03 and  ACCEPT_MASKMSG_07 within 20 i_can_clk cycles starting with the rising edge of i_can_clk recognizing i_uaf3  as high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall perform the actions in ACCEPT_MASKMSG_04 and  ACCEPT_MASKMSG_08 within 20 i_can_clk cycles starting with the rising edge of i_can_clk recognizing i_uaf4 as high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If i_uaf1,2,3 and 4 are low the module shall set o_acfbsy shall set low.  </t>
+  </si>
+  <si>
+    <t>If i_uaf1,2,3, or 4 is high the module shall set o_acfbsy high</t>
+  </si>
+  <si>
+    <t>REG</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall implement a unique full flag for indicating Internal registers1 contains new content.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall implement a unique full flag for indicating Internal registers4 contains new content.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall implement a unique full flag for indicating Internal registers3 contains new content.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall implement a unique full flag for indicating Internal registers2 contains new content.   </t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_02</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_03</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_04</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_05</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_06</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_07</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_08</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_09</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_10</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_11</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_12</t>
+  </si>
+  <si>
+    <t>FSM</t>
+  </si>
+  <si>
+    <t>ACCEPT_FSM_01</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register1 with size [31:0]</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register2 with size [31:0]</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register3 with size [31:0]</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register4 with size [31:0]</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register5 with size [31:0]</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register6 with size [31:0]</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register7 with size [31:0]</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register8 with size [31:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall transition from FSM state IDLE to state ACCEPTMESSAGE if internal register9 full flag is high and full flags internal registers1-4 full flags are low.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall transition from FSM state IDLE to state PROCESSING if internal registers9 full flag is high and any of internal registers1-4 full flags are high.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall transition from FSM state PROCESSING to state ACCEPTMESSAGE if contents of any of internal registers1-4 contents is equal to contents of internal registers5-8 in previous state IDLE.  </t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state PROCESSING to state DISCARDMESSAGE if contents of all internal register1-4 that had their full flag asserted in IDLE do not match the contents of any of the corresponding internal registers5-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall establish that the FSM may only transition to FSM state PROCESSING from FSM state IDLE.  </t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state ACCEPTMESSAGE to IDLE on next i_sys_clk rising edge after entering state ACCEPTMESSAGE</t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state DISCARDMESSAGE to IDLE on next i_sys_clk rising edge after entering state DISCARDMESSAGE</t>
+  </si>
+  <si>
+    <t>ACCEPT_FSM_02</t>
+  </si>
+  <si>
+    <t>ACCEPT_FSM_03</t>
+  </si>
+  <si>
+    <t>ACCEPT_FSM_04</t>
+  </si>
+  <si>
+    <t>ACCEPT_FSM_05</t>
+  </si>
+  <si>
+    <t>ACCEPT_FSM_06</t>
+  </si>
+  <si>
+    <t>ACCEPT_FSM_07</t>
+  </si>
+  <si>
+    <t>The module shall implement internal register9 with size [127:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall implement a unique full flag for indicating Internal registers9 contains new content.   </t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_13</t>
+  </si>
+  <si>
+    <t>ACCEPT_REG_14</t>
+  </si>
+  <si>
+    <t>ACCEPT_REC_02</t>
+  </si>
+  <si>
+    <t>If i_can_ready is high the module shall accept i_rx_message[127:0] on the next rising edge of i_can_clk and mask the contents according to ACCEPT_MASKMSG_01-08 before storing the result(s) in internal register(s) for filtering by ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall not insert data into any of the internal registers5-8 unless the data is different than the current contents.  </t>
   </si>
 </sst>
 </file>
@@ -270,7 +492,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -394,11 +616,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -432,10 +694,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,7 +1045,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,32 +1167,32 @@
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="20"/>
     </row>
     <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="20"/>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="20"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="20"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="20"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -916,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055E712C-2DEB-9048-A84E-E3F1D6680CEE}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,200 +1241,568 @@
       <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>29</v>
+      <c r="D2" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="19"/>
+      <c r="C3" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="B4" s="30"/>
       <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>33</v>
+      <c r="B6" s="12"/>
+      <c r="C6" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
-      <c r="B7" s="11"/>
+      <c r="B7" s="28" t="s">
+        <v>39</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
-      <c r="B8" s="11"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>56</v>
+      <c r="B9" s="29"/>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
-      <c r="B10" s="13" t="s">
-        <v>43</v>
-      </c>
+      <c r="B10" s="29"/>
       <c r="C10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>55</v>
+      <c r="B15" s="29"/>
+      <c r="C15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
-      <c r="B16" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>63</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="2" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="7" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="14"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="14"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="14"/>
+      <c r="B31" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="14"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
+      <c r="B35" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="14"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="14"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="14"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="14"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="14"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="14"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="14"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="14"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="14"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" s="34" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A2:A19"/>
+  <mergeCells count="8">
+    <mergeCell ref="B35:B48"/>
+    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="A2:A55"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B18"/>
+    <mergeCell ref="B19:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B2:B4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CAN2-30 Tx Priority Logic req rev2
</commit_message>
<xml_diff>
--- a/CAN_Controller_Requirements_ColinFritz.xlsx
+++ b/CAN_Controller_Requirements_ColinFritz.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfritz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfritz/my_repos/CAN_Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641C8AB4-8A81-A947-8892-BEDD012E21D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747A7F9B-8EE4-7846-B9EA-A6778B138DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="460" windowWidth="22400" windowHeight="18680" activeTab="1" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
+    <workbookView xWindow="3780" yWindow="460" windowWidth="28880" windowHeight="18680" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tx_Priority_Logic" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>TxPL_SEND_02</t>
   </si>
   <si>
-    <t>TxPL_SEND_03</t>
-  </si>
-  <si>
     <t>TxPL_REC_03</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>The module shall set o_rx_fifo_w_data[127:0] to i_rx_message[127:0] in FSM state ACCEPTMESSAGE</t>
+  </si>
+  <si>
+    <t>TxPL_SEND_01</t>
   </si>
 </sst>
 </file>
@@ -531,6 +531,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -549,18 +556,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5DD9F9-33F5-AB4F-8754-0782077CDA3E}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,7 +908,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -918,83 +918,83 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="15" t="s">
-        <v>49</v>
+      <c r="A3" s="23"/>
+      <c r="B3" s="18" t="s">
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="7" t="s">
+    <row r="8" spans="1:4" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1034,7 +1034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA590136-552A-8248-906B-60BCF433D416}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
@@ -1058,408 +1058,408 @@
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="23"/>
+      <c r="B5" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="23"/>
+      <c r="B7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="7" t="s">
+      <c r="D8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D13" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
-      <c r="B7" s="15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="23"/>
+      <c r="B16" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="2" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="7" t="s">
+      <c r="D21" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="23"/>
+      <c r="B25" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="15" t="s">
+      <c r="D25" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="2" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="2" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="2" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="2" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="2" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="2" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="22" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D34" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="21"/>
-    </row>
-    <row r="34" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="23" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D35" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="2" t="s">
+    <row r="39" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="7" t="s">
+      <c r="D39" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
     <mergeCell ref="B25:B39"/>
     <mergeCell ref="A2:A39"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B15"/>
     <mergeCell ref="B16:B24"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CAN2-30 rev4 of acceptance filter requirements
</commit_message>
<xml_diff>
--- a/CAN_Controller_Requirements_ColinFritz.xlsx
+++ b/CAN_Controller_Requirements_ColinFritz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfritz/my_repos/CAN_Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747A7F9B-8EE4-7846-B9EA-A6778B138DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4923EE-3996-A148-83AA-31FBC66B945B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="460" windowWidth="28880" windowHeight="18680" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
+    <workbookView xWindow="1560" yWindow="460" windowWidth="34120" windowHeight="18680" activeTab="1" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tx_Priority_Logic" sheetId="1" r:id="rId1"/>
@@ -261,30 +261,6 @@
     <t xml:space="preserve">The module shall perform bitwise AND operation in ACCEPT_MASKMSG_01-04 with i_afmr1-4[31] of the first signal aligned with the i_rx_message[127] bit of the second signal and so on down to position [0] of both. </t>
   </si>
   <si>
-    <t>The module shall set mask_msg_four[31:0] logic low if i_uaf4 is logic low</t>
-  </si>
-  <si>
-    <t>The module shall set mask_msg_three[31:0] logic low if i_uaf3 is logic low</t>
-  </si>
-  <si>
-    <t>The module shall set mask_msg_two[31:0] logic low if i_uaf2 is logic low</t>
-  </si>
-  <si>
-    <t>The module shall set mask_msg_one[31:0] logic low if i_uaf1 is logic low</t>
-  </si>
-  <si>
-    <t>The module shall set mask_id_one[31:0] logic low if i_uaf1 is logic low</t>
-  </si>
-  <si>
-    <t>The module shall set mask_id_four[31:0] logic low if i_uaf4 is logic low</t>
-  </si>
-  <si>
-    <t>The module shall set mask_id_three[31:0] logic low if i_uaf3 is logic low</t>
-  </si>
-  <si>
-    <t>The module shall set mask_id_two[31:0] logic low if i_uaf2  is logic low</t>
-  </si>
-  <si>
     <t>The module shall perform bitwise logical AND operation on i_afir1[31:0] with i_afmr1[31:0] and name the result mask_id_one[31:0] if i_uaf1 is logic high</t>
   </si>
   <si>
@@ -309,27 +285,6 @@
     <t>The module shall transition FSM from state IDLE to state PROCESSING if can_ready_synched is logic high</t>
   </si>
   <si>
-    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if mask_id_one[31:0] is not logic low and mask_msg_one[31:0] is not logic low and i_uaf1 is logic high and mask_id_one{31:0] is bitwise equivalent to mask_msg_one[31:0}</t>
-  </si>
-  <si>
-    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if mask_id_two[31:0] is not logic low and mask_msg_two[31:0] is not logic low and i_uaf2 is logic high and mask_id_two{31:0] is bitwise equivalent to mask_msg_two[31:0}</t>
-  </si>
-  <si>
-    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if mask_id_three[31:0] is not logic low and mask_msg_three[31:0] is not logic low and i_uaf3 is logic high and mask_id_three{31:0] is bitwise equivalent to mask_msg_three[31:0}</t>
-  </si>
-  <si>
-    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if mask_id_four[31:0] is not logic low and mask_msg_four[31:0] is not logic low and i_uaf4 is logic high and mask_id_four{31:0] is bitwise equivalent to mask_msg_four[31:0}</t>
-  </si>
-  <si>
-    <t>The module shall transition FSM from state PROCESSING to state DISCARDMESSAGE if i_uaf1, i_uaf2, i_uaf3, i_uaf4 are all logic low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall transition FSM from state PROCESSING to state DISCARDMESSAGE if ( (mask_id_one[31:0] bitwise equivalent w/ mask_msg_one[31:0]) logical OR (mask_id_two[31:0] bitwise equivalent w/ mask_msg_two[31:0]) logical OR (mask_id_three[31:0] bitwise equivalent w/ mask_msg_three[31:0]) logical OR (mask_id_four[31:0] bitwise equivalent w/ mask_msg_four[31:0]) ) is False.  </t>
-  </si>
-  <si>
-    <t>The module shall transition FSM from state PROCESSING to state DISCARDMESSAGE if mask_id_one[31:0], mask_id_two[31:0], mask_id_three[31:0], mask_id_four[31:0], mask_msg_one[31:0], mask_msg_two[31:0], mask_msg_three[31:0], and mask_msg_four[31:0] are all logic low</t>
-  </si>
-  <si>
     <t>ACCEPT_FSM_13</t>
   </si>
   <si>
@@ -352,6 +307,51 @@
   </si>
   <si>
     <t>TxPL_SEND_01</t>
+  </si>
+  <si>
+    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if 1. mask_id_one[31:0] is not "00000000000000000000000000000000" and 2.  mask_msg_one[31:0] is not '00000000000000000000000000000000'  and 3.i_uaf1 is logic high and 4. mask_id_one{31:0] is bitwise equivalent to mask_msg_one[31:0}</t>
+  </si>
+  <si>
+    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if 1. i_uaf1 logic low and 2.i_uaf2 logic low and 3.i_uaf3 logic low and 4.i_uaf4 logic low</t>
+  </si>
+  <si>
+    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if 1. mask_id_one[31:0] is "00000000000000000000000000000000"  and 2.mask_id_two[31:0] "00000000000000000000000000000000" and 3.mask_id_three[31:0] is "00000000000000000000000000000000" and 4.mask_id_four[31:0] is "00000000000000000000000000000000" and 5.mask_msg_one[31:0] is "00000000000000000000000000000000" 6.mask_msg_two[31:0] is "00000000000000000000000000000000" 7.mask_msg_three[31:0] is "00000000000000000000000000000000" and 8.mask_msg_four[31:0] is "00000000000000000000000000000000"</t>
+  </si>
+  <si>
+    <t>The module shall transition FSM from state PROCESSING to state DISCARDMESSAGE if none of the conditional statements in ACCEPT_FSM_03-08 evaluate to True</t>
+  </si>
+  <si>
+    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if 1.  mask_id_two[31:0] is not "00000000000000000000000000000000" and 2.  mask_msg_two[31:0] is not "00000000000000000000000000000000" and 3.i_uaf2 is logic high and 4. mask_id_two{31:0] is bitwise equivalent to mask_msg_two[31:0]</t>
+  </si>
+  <si>
+    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if 1. mask_id_three[31:0] is not "00000000000000000000000000000000" and 2. mask_msg_three[31:0] is not "00000000000000000000000000000000" and 3.i_uaf3 is logic high and 4. mask_id_three{31:0] is bitwise equivalent to mask_msg_three[31:0]</t>
+  </si>
+  <si>
+    <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if 1. mask_id_four[31:0] is not "00000000000000000000000000000000" and 2. mask_msg_four[31:0] is not "00000000000000000000000000000000" and 3. i_uaf4 is logic high and 4.mask_id_four[31:0] is bitwise equivalent to mask_msg_four[31:0]</t>
+  </si>
+  <si>
+    <t>The module shall set mask_id_one[31:0] to "00000000000000000000000000000000" if i_uaf1 is logic low</t>
+  </si>
+  <si>
+    <t>The module shall set mask_id_two[31:0] to "00000000000000000000000000000000" if i_uaf2  is logic low</t>
+  </si>
+  <si>
+    <t>The module shall set mask_id_three[31:0] to "00000000000000000000000000000000" if i_uaf3 is logic low</t>
+  </si>
+  <si>
+    <t>The module shall set mask_id_four[31:0] to "00000000000000000000000000000000" if i_uaf4 is logic low</t>
+  </si>
+  <si>
+    <t>The module shall set mask_msg_one[31:0] to "00000000000000000000000000000000" if i_uaf1 is logic low</t>
+  </si>
+  <si>
+    <t>The module shall set mask_msg_two[31:0] to "00000000000000000000000000000000" if i_uaf2 is logic low</t>
+  </si>
+  <si>
+    <t>The module shall set mask_msg_three[31:0] to "00000000000000000000000000000000" if i_uaf3 is logic low</t>
+  </si>
+  <si>
+    <t>The module shall set mask_msg_four[31:0] to "00000000000000000000000000000000" if i_uaf4 is logic low</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -531,10 +531,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -555,12 +551,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5DD9F9-33F5-AB4F-8754-0782077CDA3E}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -908,7 +898,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -922,20 +912,20 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="18" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
@@ -944,8 +934,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -956,8 +946,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -966,8 +956,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
@@ -976,8 +966,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -988,8 +978,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="13" t="s">
         <v>34</v>
       </c>
@@ -1032,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA590136-552A-8248-906B-60BCF433D416}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,10 +1052,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1076,8 +1066,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1086,8 +1076,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="7" t="s">
         <v>37</v>
       </c>
@@ -1096,8 +1086,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="16" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1108,8 +1098,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="7" t="s">
         <v>64</v>
       </c>
@@ -1118,8 +1108,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1130,8 +1120,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1140,8 +1130,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1150,8 +1140,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1160,48 +1150,48 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="7" t="s">
         <v>40</v>
       </c>
@@ -1210,252 +1200,243 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="18" t="s">
-        <v>88</v>
+      <c r="A25" s="21"/>
+      <c r="B25" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
+      <c r="D28" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
+      <c r="D29" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>94</v>
+      <c r="D30" s="15" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="15"/>
-    </row>
-    <row r="34" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="16" t="s">
+      <c r="D32" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
+      <c r="D33" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="2" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>103</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B25:B39"/>
-    <mergeCell ref="A2:A39"/>
+  <mergeCells count="6">
+    <mergeCell ref="B25:B38"/>
+    <mergeCell ref="A2:A38"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B15"/>

</xml_diff>

<commit_message>
CAN2-30 tx priority logic reqs change for matt
</commit_message>
<xml_diff>
--- a/CAN_Controller_Requirements_ColinFritz.xlsx
+++ b/CAN_Controller_Requirements_ColinFritz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfritz/my_repos/CAN_Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4923EE-3996-A148-83AA-31FBC66B945B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ECD8CB-72CC-9849-AB94-D58C2185EE25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="460" windowWidth="34120" windowHeight="18680" activeTab="1" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
+    <workbookView xWindow="4640" yWindow="460" windowWidth="28960" windowHeight="18680" xr2:uid="{3DEFB132-B4FA-6B47-A92F-7E0931A5A55D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tx_Priority_Logic" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="125">
   <si>
     <t>Function</t>
   </si>
@@ -54,30 +54,6 @@
     <t>TxPL_INIT_01</t>
   </si>
   <si>
-    <t>Initialization</t>
-  </si>
-  <si>
-    <t>TxPL_REC_02</t>
-  </si>
-  <si>
-    <t>TxPL_REC_01</t>
-  </si>
-  <si>
-    <t>Receive Data</t>
-  </si>
-  <si>
-    <t>TxPL_SEND_02</t>
-  </si>
-  <si>
-    <t>TxPL_REC_03</t>
-  </si>
-  <si>
-    <t>TxPL_PRIORITY_01</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
     <t>ACCEPT</t>
   </si>
   <si>
@@ -138,12 +114,6 @@
     <t>ACCEPT_MASKMSG_01</t>
   </si>
   <si>
-    <t>TxPL_PRIORITY_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall implement full and empty flags for indicating the occupancy of the internal register.  </t>
-  </si>
-  <si>
     <t>ACCEPT_INIT_02</t>
   </si>
   <si>
@@ -180,30 +150,6 @@
     <t>ACCEPT_FSM_07</t>
   </si>
   <si>
-    <t>SEND</t>
-  </si>
-  <si>
-    <t>The module shall contain an internal register for accepting data from TX FIFO and TXHPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall set o_hpb_r_en and o_fifo_r_en low if i_hpb_w_en is low and  i_reset is low and i_tx_empty is high </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall pulse o_fifo_r_en (low to high to low) for one i_sys_clk period if i_hpb_w_en is low and i_reset is low and i_tx_empty Is low the internal register is empty  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall pulse o_hpb_r_en (low to high to low) for one i_sys_clk period if i_hpb_w_en is high and i_reset is low  and the internal register is empty </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall set o_send_en to logic low if i_busy_can is high </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall pulse o_send_en continually as long as the modules internal register contains data if i_busy_can is logic low and i_reset is logic low </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The module shall set o_fifo_r_en and o_hpb_r_en and o_send_en and o_send_data[127:0]  to logic low  If i_reset is logic high </t>
-  </si>
-  <si>
     <t>ACCEPT_FSM_08</t>
   </si>
   <si>
@@ -306,9 +252,6 @@
     <t>The module shall set o_rx_fifo_w_data[127:0] to i_rx_message[127:0] in FSM state ACCEPTMESSAGE</t>
   </si>
   <si>
-    <t>TxPL_SEND_01</t>
-  </si>
-  <si>
     <t>The module shall transition FSM from state PROCESSING to state ACCEPTMESSAGE if 1. mask_id_one[31:0] is not "00000000000000000000000000000000" and 2.  mask_msg_one[31:0] is not '00000000000000000000000000000000'  and 3.i_uaf1 is logic high and 4. mask_id_one{31:0] is bitwise equivalent to mask_msg_one[31:0}</t>
   </si>
   <si>
@@ -352,6 +295,120 @@
   </si>
   <si>
     <t>The module shall set mask_msg_four[31:0] to "00000000000000000000000000000000" if i_uaf4 is logic low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall set o_fifo_r_en and o_hpb_r_en and o_send_en and o_send_data[127:0]  to "00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000"  If i_reset is logic high </t>
+  </si>
+  <si>
+    <t>FSM</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_01</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_02</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_03</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_04</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_05</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_06</t>
+  </si>
+  <si>
+    <t>TxPL_INIT_02</t>
+  </si>
+  <si>
+    <t>The module shall initialize FSM to state IDLE if i_reset is logic high</t>
+  </si>
+  <si>
+    <t>The module shall set o_hpb_r_en logic high in FSM state HPB_PULL_DATA</t>
+  </si>
+  <si>
+    <t>The module shall set o_fifo_r_en logic high in FSM state FIFO_PULL_DATA</t>
+  </si>
+  <si>
+    <t>The module shall set o_send_en high in FSM state HPB_SEND_DATA if i_busy_can is logic low</t>
+  </si>
+  <si>
+    <t>The module shall set o_send_en high in FSM state FIFO_SEND_DATA if i_busy_can is logic low</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_07</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_08</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_09</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_10</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_11</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_12</t>
+  </si>
+  <si>
+    <t>The module shall set i_hpb_data[127:0] to o_send_data[127:0] in FSM state HPB_SEND_DATA</t>
+  </si>
+  <si>
+    <t>The module shall set i_fifo_data[127:0] to o_send_data[127:0] in FSM state FIFO_SEND_DATA</t>
+  </si>
+  <si>
+    <t>The module shall set o_hpb_r_en and o_fifo_r_en and o_send_en to logic low in FSM state IDLE</t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state IDLE to FSM state HPB_PULL_DATA if i_hpb_w_en is logic low</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_13</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_14</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_15</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_16</t>
+  </si>
+  <si>
+    <t>TxPL_FSM_17</t>
+  </si>
+  <si>
+    <t>The module shall implement FSM with states IDLE, HPB_PULL_DATA, FIFO_PULL_DATA, WAIT_FOR_FIFO_DATA, WAIT_FOR_HPB_DATA, HPB_SEND_DATA, FIFO_SEND_DATA</t>
+  </si>
+  <si>
+    <t>The module shall set o_fifo_r_en to logic low in FSM state WAIT_FOR_FIFO_DATA</t>
+  </si>
+  <si>
+    <t>The module shall set o_hpb_r_en to logic low in FSM state WAIT_FOR_HPB_DATA</t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state HPB_PULL_DATA to FSM state WAIT_FOR_HPB_DATA under all conditions</t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state FIFO_PULL_DATA to FSM state WAIT_FOR_FIFO_DATA under all conditions</t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state WAIT_FOR_HPB_DATA to FSM state HPB_SEND_DATA under all conditions</t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state WAIT_FOR_FIFO_DATA  to FSM state FIFO_SEND_DATA under all conditions</t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM states HPB_SEND_DATA and FIFO_SEND_DATA to FSM state IDLE under all conditions</t>
+  </si>
+  <si>
+    <t>The module shall transition from FSM state IDLE to FSM state FIFO_PULL_DATA If i_tx_empty is logic low and i_hpb_w_en is logic high</t>
   </si>
 </sst>
 </file>
@@ -519,27 +576,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -549,9 +593,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5DD9F9-33F5-AB4F-8754-0782077CDA3E}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,143 +930,227 @@
     <col min="1" max="1" width="27" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="156.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="235.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="16" t="s">
-        <v>48</v>
-      </c>
+      <c r="D2" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
+      <c r="D5" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-    </row>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="17"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="17"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B8:B9"/>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B20"/>
+    <mergeCell ref="A2:A20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1024,7 +1161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA590136-552A-8248-906B-60BCF433D416}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -1038,399 +1175,399 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>61</v>
+      <c r="D1" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+      <c r="B16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="D21" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D23" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="17"/>
+      <c r="B25" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="s">
+    <row r="38" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="D38" s="7" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
-      <c r="B16" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>